<commit_message>
large variety of changes
</commit_message>
<xml_diff>
--- a/data-raw/animals/animalBreakpointslistRaw.xlsx
+++ b/data-raw/animals/animalBreakpointslistRaw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/ISIMIPData/data-raw/animals/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1A02BF9-531D-D84E-A3BA-781DBA8E18BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2839845-F9C0-6348-B9EE-733A1C74219C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15880" yWindow="9800" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7820" yWindow="3540" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="animalBreakpointslistRaw" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>species</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>chicken</t>
+  </si>
+  <si>
+    <t>maximum</t>
   </si>
 </sst>
 </file>
@@ -911,15 +914,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:E8"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -935,8 +938,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -952,8 +958,11 @@
       <c r="E2" s="1">
         <v>89</v>
       </c>
+      <c r="F2" s="1">
+        <v>115</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -969,8 +978,11 @@
       <c r="E3" s="1">
         <v>25.6</v>
       </c>
+      <c r="F3" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -986,8 +998,11 @@
       <c r="E4" s="1">
         <v>89</v>
       </c>
+      <c r="F4" s="1">
+        <v>115</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1003,8 +1018,11 @@
       <c r="E5" s="1">
         <v>62</v>
       </c>
+      <c r="F5" s="1">
+        <v>100</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1020,8 +1038,11 @@
       <c r="E6" s="1">
         <v>30</v>
       </c>
+      <c r="F6" s="1">
+        <v>70</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1037,8 +1058,11 @@
       <c r="E7" s="1">
         <v>30</v>
       </c>
+      <c r="F7" s="1">
+        <v>50</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1053,6 +1077,9 @@
       </c>
       <c r="E8" s="1">
         <v>30</v>
+      </c>
+      <c r="F8" s="1">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>